<commit_message>
Fix BigDecimal and number percentage display.
</commit_message>
<xml_diff>
--- a/excel/user_writer.xlsx
+++ b/excel/user_writer.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="12">
   <si>
     <t/>
   </si>
@@ -26,13 +26,10 @@
     <t>2019-10-10</t>
   </si>
   <si>
-    <t>0.1</t>
-  </si>
-  <si>
     <t>lyan2@ebay.com</t>
   </si>
   <si>
-    <t>2019-10-10 17:31:23</t>
+    <t>2019-10-10 17:55:26</t>
   </si>
   <si>
     <t>Linus</t>
@@ -50,13 +47,7 @@
     <t>false</t>
   </si>
   <si>
-    <t>17:31:23</t>
-  </si>
-  <si>
-    <t>2019-10-10 17:31:24</t>
-  </si>
-  <si>
-    <t>17:31:24</t>
+    <t>17:55:26</t>
   </si>
 </sst>
 </file>
@@ -160,6 +151,14 @@
       <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true" horizontal="right"/>
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true"/>
+      <protection locked="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
@@ -232,14 +231,6 @@
       <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-      <protection locked="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
-      <alignment wrapText="true"/>
-      <protection locked="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
@@ -248,6 +239,10 @@
       <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true" horizontal="right"/>
+      <protection locked="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
@@ -284,10 +279,6 @@
       <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-      <protection locked="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
@@ -296,6 +287,10 @@
       <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true" horizontal="right"/>
+      <protection locked="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
@@ -310,10 +305,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
-      <protection locked="false"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
-      <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
@@ -353,6 +344,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="3" max="3" width="8.375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="8.375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.4375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="8.375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.9140625" customWidth="true" bestFit="true"/>
@@ -361,155 +353,160 @@
     <col min="7" max="7" width="8.375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="8.375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="8.375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="8.375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="8.375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="9.15625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="7">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s" s="10">
+      <c r="A1" t="s" s="8">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="11">
         <v>1</v>
       </c>
       <c r="C1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="9">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s" s="11">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s" s="8">
+      <c r="D1" t="s" s="10">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s" s="6">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s" s="9">
         <v>1</v>
       </c>
       <c r="H1" t="s" s="12">
         <v>1</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" t="s" s="4">
         <v>1</v>
       </c>
       <c r="K1" t="s" s="13">
         <v>1</v>
       </c>
-      <c r="L1" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="M1" t="s" s="6">
+      <c r="L1" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="25">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="31">
-        <v>10</v>
+      <c r="A2" t="s" s="27">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s" s="33">
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="15">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="29">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="21">
+      <c r="D2" t="s" s="31">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="23">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="G2" t="s" s="29">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s" s="35">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s" s="19">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s" s="37">
+        <v>11</v>
+      </c>
+      <c r="L2" t="n" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="M2" t="s" s="25">
         <v>5</v>
-      </c>
-      <c r="F2" s="33"/>
-      <c r="G2" t="s" s="27">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s" s="35">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s" s="17">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s" s="37">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s" s="19">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s" s="23">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="43">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="46">
-        <v>10</v>
+      <c r="A3" t="s" s="44">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="47">
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="38">
         <v>2</v>
       </c>
-      <c r="D3" t="s" s="45">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s" s="41">
+      <c r="D3" t="s" s="46">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="42">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="G3" t="s" s="45">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s" s="48">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s" s="40">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s" s="49">
+        <v>11</v>
+      </c>
+      <c r="L3" t="n" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="M3" t="s" s="43">
         <v>5</v>
-      </c>
-      <c r="F3" s="47"/>
-      <c r="G3" t="s" s="44">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s" s="48">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s" s="39">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s" s="49">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s" s="40">
-        <v>4</v>
-      </c>
-      <c r="M3" t="s" s="42">
-        <v>13</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="55">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s" s="58">
-        <v>10</v>
+      <c r="A4" t="s" s="56">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="59">
+        <v>9</v>
       </c>
       <c r="C4" t="s" s="50">
         <v>2</v>
       </c>
-      <c r="D4" t="s" s="57">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s" s="53">
+      <c r="D4" t="s" s="58">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="54">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n" s="51">
+        <v>1.0</v>
+      </c>
+      <c r="G4" t="s" s="57">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s" s="60">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s" s="52">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s" s="61">
+        <v>11</v>
+      </c>
+      <c r="L4" t="n" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="M4" t="s" s="55">
         <v>5</v>
-      </c>
-      <c r="F4" s="59"/>
-      <c r="G4" t="s" s="56">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s" s="60">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s" s="51">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s" s="61">
-        <v>14</v>
-      </c>
-      <c r="L4" t="s" s="52">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s" s="54">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split map, list and pojo sheet reader.
</commit_message>
<xml_diff>
--- a/excel/user_writer.xlsx
+++ b/excel/user_writer.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="11">
   <si>
     <t/>
   </si>
@@ -20,16 +20,13 @@
     <t>默认标题</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>2019-10-11</t>
   </si>
   <si>
     <t>lyan2@ebay.com</t>
   </si>
   <si>
-    <t>2019-10-11 11:06:24</t>
+    <t>2019-10-11 11:12:10</t>
   </si>
   <si>
     <t>Linus</t>
@@ -47,7 +44,7 @@
     <t>false</t>
   </si>
   <si>
-    <t>11:06:24</t>
+    <t>11:12:10</t>
   </si>
 </sst>
 </file>
@@ -143,14 +140,6 @@
       <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-      <protection locked="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
-      <alignment wrapText="true"/>
-      <protection locked="false"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
       <alignment wrapText="true" horizontal="right"/>
       <protection locked="false"/>
@@ -159,6 +148,14 @@
       <alignment wrapText="true"/>
       <protection locked="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true" horizontal="right"/>
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true"/>
+      <protection locked="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
@@ -235,14 +232,14 @@
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-      <protection locked="false"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
       <alignment wrapText="true" horizontal="right"/>
       <protection locked="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true" horizontal="right"/>
+      <protection locked="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
@@ -283,8 +280,8 @@
       <alignment wrapText="true" horizontal="center"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyNumberFormat="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
+      <alignment wrapText="true" horizontal="right"/>
       <protection locked="false"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false">
@@ -397,116 +394,116 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s" s="33">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s" s="15">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="n" s="15">
+        <v>30.0</v>
       </c>
       <c r="D2" t="s" s="31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n" s="17">
         <v>1.0</v>
       </c>
       <c r="G2" t="s" s="29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s" s="35">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s" s="19">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s" s="37">
         <v>10</v>
-      </c>
-      <c r="I2" t="s" s="19">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s" s="37">
-        <v>11</v>
       </c>
       <c r="L2" t="n" s="21">
         <v>0.1</v>
       </c>
       <c r="M2" t="s" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s" s="47">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s" s="38">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="n" s="38">
+        <v>30.0</v>
       </c>
       <c r="D3" t="s" s="46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s" s="42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n" s="39">
         <v>1.0</v>
       </c>
       <c r="G3" t="s" s="45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s" s="48">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s" s="40">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s" s="49">
         <v>10</v>
-      </c>
-      <c r="I3" t="s" s="40">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s" s="49">
-        <v>11</v>
       </c>
       <c r="L3" t="n" s="41">
         <v>0.1</v>
       </c>
       <c r="M3" t="s" s="43">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="56">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s" s="59">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="50">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C4" t="n" s="50">
+        <v>30.0</v>
       </c>
       <c r="D4" t="s" s="58">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s" s="54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n" s="51">
         <v>1.0</v>
       </c>
       <c r="G4" t="s" s="57">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s" s="60">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s" s="52">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s" s="61">
         <v>10</v>
-      </c>
-      <c r="I4" t="s" s="52">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s" s="61">
-        <v>11</v>
       </c>
       <c r="L4" t="n" s="53">
         <v>0.1</v>
       </c>
       <c r="M4" t="s" s="55">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>